<commit_message>
Just about finished communications db driver
</commit_message>
<xml_diff>
--- a/workbooks/CommsDatabase.xlsx
+++ b/workbooks/CommsDatabase.xlsx
@@ -2,20 +2,117 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter\Documents\NetBeansProjects\DisasterResponseTradeStudy\workbooks\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18750" windowHeight="12690"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Communication" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171026"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Category Name</t>
+  </si>
+  <si>
+    <t>Range (km)</t>
+  </si>
+  <si>
+    <t>Cost Ranking</t>
+  </si>
+  <si>
+    <t>Terrain 1</t>
+  </si>
+  <si>
+    <t>Terrain 2</t>
+  </si>
+  <si>
+    <t>Terrain 3</t>
+  </si>
+  <si>
+    <t>Terrain 4</t>
+  </si>
+  <si>
+    <t>Disaster Effect</t>
+  </si>
+  <si>
+    <t>4,9</t>
+  </si>
+  <si>
+    <t>Data Rate (Mbps)</t>
+  </si>
+  <si>
+    <t>Weight (kg)</t>
+  </si>
+  <si>
+    <t>Platform Restrictions</t>
+  </si>
+  <si>
+    <t>Short Range</t>
+  </si>
+  <si>
+    <t>6,13</t>
+  </si>
+  <si>
+    <t>Satellite VGC</t>
+  </si>
+  <si>
+    <t>5,6,7</t>
+  </si>
+  <si>
+    <t>Satellite Internet</t>
+  </si>
+  <si>
+    <t>Omni-Directional Microwave</t>
+  </si>
+  <si>
+    <t>2,13</t>
+  </si>
+  <si>
+    <t>2,6,12,13</t>
+  </si>
+  <si>
+    <t>Hybrid Microwave</t>
+  </si>
+  <si>
+    <t>10,11,12,13,14,15</t>
+  </si>
+  <si>
+    <t>PtP Microwave</t>
+  </si>
+  <si>
+    <t>LTE Cellular</t>
+  </si>
+  <si>
+    <t>3G Cellular</t>
+  </si>
+  <si>
+    <t>BLOS</t>
+  </si>
+  <si>
+    <t>1,2,3,4,5,6,7,8,9</t>
+  </si>
+  <si>
+    <t>2,6,12</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -29,12 +126,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -49,8 +152,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -144,6 +257,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -179,6 +309,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -331,12 +478,389 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:N1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" style="3" customWidth="1"/>
+    <col min="8" max="14" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2</v>
+      </c>
+      <c r="J2" s="4">
+        <v>13</v>
+      </c>
+      <c r="K2" s="4">
+        <v>13</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="4"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1">
+        <v>8000</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4">
+        <v>6</v>
+      </c>
+      <c r="L3" s="4">
+        <v>6</v>
+      </c>
+      <c r="M3" s="4">
+        <v>6</v>
+      </c>
+      <c r="N3" s="4"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1">
+        <v>8000</v>
+      </c>
+      <c r="D4" s="1">
+        <v>25</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2</v>
+      </c>
+      <c r="F4" s="1">
+        <v>10</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4">
+        <v>6</v>
+      </c>
+      <c r="L4" s="4">
+        <v>6</v>
+      </c>
+      <c r="M4" s="4">
+        <v>6</v>
+      </c>
+      <c r="N4" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="1">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1">
+        <v>40</v>
+      </c>
+      <c r="E5" s="1">
+        <v>2</v>
+      </c>
+      <c r="F5" s="1">
+        <v>3</v>
+      </c>
+      <c r="J5" s="4">
+        <v>13</v>
+      </c>
+      <c r="K5" s="4">
+        <v>13</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N5" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="1">
+        <v>70</v>
+      </c>
+      <c r="D6" s="1">
+        <v>40</v>
+      </c>
+      <c r="E6" s="1">
+        <v>3</v>
+      </c>
+      <c r="F6" s="1">
+        <v>5</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4">
+        <v>13</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N6" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="1">
+        <v>160</v>
+      </c>
+      <c r="D7" s="1">
+        <v>40</v>
+      </c>
+      <c r="E7" s="1">
+        <v>4</v>
+      </c>
+      <c r="F7" s="1">
+        <v>10</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N7" s="4"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="1">
+        <v>8</v>
+      </c>
+      <c r="D8" s="1">
+        <v>300</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4">
+        <v>6</v>
+      </c>
+      <c r="N8" s="4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="1">
+        <v>8</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4">
+        <v>6</v>
+      </c>
+      <c r="N9" s="4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="1">
+        <v>200</v>
+      </c>
+      <c r="D10" s="1">
+        <v>22</v>
+      </c>
+      <c r="E10" s="1">
+        <v>5</v>
+      </c>
+      <c r="F10" s="1">
+        <v>70</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C22" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finished DB Drivers and Platform filter.
</commit_message>
<xml_diff>
--- a/workbooks/CommsDatabase.xlsx
+++ b/workbooks/CommsDatabase.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>ID</t>
   </si>
@@ -86,9 +86,6 @@
     <t>2,13</t>
   </si>
   <si>
-    <t>2,6,12,13</t>
-  </si>
-  <si>
     <t>Hybrid Microwave</t>
   </si>
   <si>
@@ -111,6 +108,9 @@
   </si>
   <si>
     <t>2,6,12</t>
+  </si>
+  <si>
+    <t>6,12</t>
   </si>
 </sst>
 </file>
@@ -481,7 +481,7 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:N1048576"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,8 +560,8 @@
       <c r="L2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="4" t="s">
-        <v>14</v>
+      <c r="M2" s="4">
+        <v>6</v>
       </c>
       <c r="N2" s="4"/>
     </row>
@@ -664,7 +664,7 @@
         <v>19</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="N5" s="4">
         <v>4</v>
@@ -675,7 +675,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="1">
         <v>70</v>
@@ -690,7 +690,7 @@
         <v>5</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4">
@@ -700,7 +700,7 @@
         <v>19</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="N6" s="4">
         <v>4</v>
@@ -711,7 +711,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="1">
         <v>160</v>
@@ -726,7 +726,7 @@
         <v>10</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
@@ -734,7 +734,7 @@
         <v>19</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="N7" s="4"/>
     </row>
@@ -743,7 +743,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" s="1">
         <v>8</v>
@@ -772,7 +772,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="1">
         <v>8</v>
@@ -801,7 +801,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" s="1">
         <v>200</v>
@@ -816,12 +816,12 @@
         <v>70</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M10" s="4" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
Updated to be able to take custom defined attributes and cleaned up database drivers to use generics and abstracts better
</commit_message>
<xml_diff>
--- a/workbooks/CommsDatabase.xlsx
+++ b/workbooks/CommsDatabase.xlsx
@@ -13,6 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="Communication" sheetId="2" r:id="rId1"/>
+    <sheet name="Communications Description" sheetId="3" r:id="rId2"/>
+    <sheet name="Supported Data Type" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171026"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="45">
   <si>
     <t>ID</t>
   </si>
@@ -111,13 +113,61 @@
   </si>
   <si>
     <t>6,12</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Col Number</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Sorting</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>km</t>
+  </si>
+  <si>
+    <t>java.lang.String</t>
+  </si>
+  <si>
+    <t>java.lang.Integer</t>
+  </si>
+  <si>
+    <t>java.lang.Double</t>
+  </si>
+  <si>
+    <t>ASCENDING</t>
+  </si>
+  <si>
+    <t>DESCENDING</t>
+  </si>
+  <si>
+    <t>Data Types</t>
+  </si>
+  <si>
+    <t>Sort Orders</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Rate </t>
+  </si>
+  <si>
+    <t>Mbps</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,8 +175,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -136,6 +194,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -152,7 +222,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -163,6 +233,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -480,8 +559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,4 +942,131 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" style="5" customWidth="1"/>
+    <col min="2" max="3" width="15.28515625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="5">
+        <v>2</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Supported Data Type'!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D3</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.42578125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>